<commit_message>
docs: update req spec
</commit_message>
<xml_diff>
--- a/sample_repo/doc/dev/RequirementsSpecification.xlsx
+++ b/sample_repo/doc/dev/RequirementsSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\foox\workspace\documentation_templates\sample_repo\doc\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37886619-9099-41C9-97C6-B324D3DF7A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDB5348-E432-4D5F-A35A-F45BCB95BF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="6495" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,31 +310,16 @@
     <t>&lt;内容&gt;</t>
   </si>
   <si>
-    <t>　要求</t>
-  </si>
-  <si>
     <t>&lt;カテゴリID.連番数値&gt;</t>
   </si>
   <si>
     <t>理由</t>
   </si>
   <si>
-    <t>　　　仕様グループ</t>
-  </si>
-  <si>
     <t>&lt;要求ID-任意文字列&gt;</t>
   </si>
   <si>
-    <t>　　　　仕様</t>
-  </si>
-  <si>
     <t>&lt;仕様グループID.連番数値&gt;</t>
-  </si>
-  <si>
-    <t>　親要求</t>
-  </si>
-  <si>
-    <t>　　子要求</t>
   </si>
   <si>
     <t>&lt;親要求ID.連番数値&gt;</t>
@@ -567,7 +552,26 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>中</t>
+    <t>要求</t>
+  </si>
+  <si>
+    <t>仕様グループ</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>仕様</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>親要求</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>子要求</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>高</t>
   </si>
 </sst>
 </file>
@@ -903,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1033,11 +1037,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,14 +1048,60 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2375,7 +2423,7 @@
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B97" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2446,24 +2494,24 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="50" t="s">
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="52"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="50"/>
     </row>
     <row r="3" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
@@ -2484,8 +2532,8 @@
       <c r="G3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="54" t="s">
-        <v>169</v>
+      <c r="H3" s="47" t="s">
+        <v>164</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>76</v>
@@ -2552,11 +2600,11 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="47" t="s">
-        <v>91</v>
+      <c r="B5" s="52" t="s">
+        <v>165</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>90</v>
@@ -2564,7 +2612,7 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="60"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
@@ -2579,9 +2627,9 @@
       <c r="T5" s="19"/>
     </row>
     <row r="6" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="48"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>90</v>
@@ -2589,7 +2637,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="H6" s="61"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
@@ -2604,7 +2652,7 @@
       <c r="T6" s="23"/>
     </row>
     <row r="7" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="49"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="25" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2660,7 @@
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
       <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="H7" s="62"/>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -2627,11 +2675,11 @@
       <c r="T7" s="27"/>
     </row>
     <row r="8" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B8" s="13" t="s">
-        <v>94</v>
+      <c r="B8" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>90</v>
@@ -2654,11 +2702,11 @@
       <c r="T8" s="15"/>
     </row>
     <row r="9" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B9" s="13" t="s">
-        <v>96</v>
+      <c r="B9" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>90</v>
@@ -2666,7 +2714,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -2714,11 +2762,11 @@
       <c r="T10" s="15"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="47" t="s">
-        <v>98</v>
+      <c r="B11" s="52" t="s">
+        <v>168</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>90</v>
@@ -2726,7 +2774,7 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -2741,9 +2789,9 @@
       <c r="T11" s="19"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="48"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>90</v>
@@ -2751,7 +2799,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
@@ -2766,7 +2814,7 @@
       <c r="T12" s="23"/>
     </row>
     <row r="13" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="25" t="s">
         <v>0</v>
       </c>
@@ -2774,7 +2822,7 @@
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
@@ -2789,11 +2837,11 @@
       <c r="T13" s="27"/>
     </row>
     <row r="14" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B14" s="47" t="s">
-        <v>99</v>
+      <c r="B14" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>90</v>
@@ -2816,9 +2864,9 @@
       <c r="T14" s="19"/>
     </row>
     <row r="15" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B15" s="48"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>90</v>
@@ -2841,7 +2889,7 @@
       <c r="T15" s="23"/>
     </row>
     <row r="16" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B16" s="49"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="25" t="s">
         <v>0</v>
       </c>
@@ -2864,11 +2912,11 @@
       <c r="T16" s="27"/>
     </row>
     <row r="17" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B17" s="13" t="s">
-        <v>94</v>
+      <c r="B17" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>90</v>
@@ -2891,11 +2939,11 @@
       <c r="T17" s="15"/>
     </row>
     <row r="18" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B18" s="13" t="s">
-        <v>96</v>
+      <c r="B18" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>90</v>
@@ -2903,7 +2951,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
@@ -2937,7 +2985,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="32" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="O19" s="33">
         <f ca="1">SQRT(SUM($P$4:OFFSET($P19,-1,0)))</f>
@@ -2962,7 +3010,7 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="32" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="O20" s="33">
         <v>0</v>
@@ -23554,42 +23602,54 @@
       <c r="T1000" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H5:H7"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <conditionalFormatting sqref="E4:F4 E10:F10">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H4 G10:H10">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AH4 I10:AH10">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>C9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C18</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(F4))), AND(ISNUMBER(F4), LEFT(CELL("format", F4))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B5 B8:B11 B14 B17:B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"カテゴリ,　要求,　親要求,　　子要求,　　　仕様グループ,　　　　仕様"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18 G9" xr:uid="{42073A2B-9420-44E9-92F6-3B2B0D0F75E0}">
       <formula1>"済"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9 H18" xr:uid="{64082CDF-C1E5-4C1A-B481-DB5D9F3AB598}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5 H11" xr:uid="{64082CDF-C1E5-4C1A-B481-DB5D9F3AB598}">
       <formula1>"高,中,低"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B18" xr:uid="{AEB3BCDC-0E4F-4A31-9D6F-6B3F7FE725A6}">
+      <formula1>"カテゴリ,要求,親要求,子要求,仕様グループ,仕様"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23658,24 +23718,24 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="50" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="50" t="s">
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="52"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="50"/>
     </row>
     <row r="3" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
@@ -23696,8 +23756,8 @@
       <c r="G3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="54" t="s">
-        <v>169</v>
+      <c r="H3" s="47" t="s">
+        <v>164</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>76</v>
@@ -23724,16 +23784,16 @@
         <v>83</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -23741,13 +23801,13 @@
         <v>88</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F4" s="41">
         <v>44929</v>
@@ -23768,23 +23828,25 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="47" t="s">
-        <v>91</v>
+      <c r="B5" s="52" t="s">
+        <v>165</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F5" s="42">
         <v>44929</v>
       </c>
       <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="60" t="s">
+        <v>170</v>
+      </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
@@ -23799,21 +23861,21 @@
       <c r="T5" s="19"/>
     </row>
     <row r="6" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="48"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F6" s="43">
         <v>44929</v>
       </c>
       <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="H6" s="61"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
@@ -23828,19 +23890,19 @@
       <c r="T6" s="23"/>
     </row>
     <row r="7" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="49"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F7" s="44">
         <v>44929</v>
       </c>
       <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="H7" s="62"/>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -23855,17 +23917,17 @@
       <c r="T7" s="27"/>
     </row>
     <row r="8" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B8" s="13" t="s">
-        <v>94</v>
+      <c r="B8" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F8" s="41">
         <v>44929</v>
@@ -23886,38 +23948,36 @@
       <c r="T8" s="15"/>
     </row>
     <row r="9" spans="2:20" ht="30" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B9" s="13" t="s">
-        <v>96</v>
+      <c r="B9" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F9" s="41">
         <v>44929</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>170</v>
-      </c>
+      <c r="H9" s="15"/>
       <c r="I9" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="M9" s="14">
         <v>0.5</v>
@@ -23934,14 +23994,14 @@
         <v>6.25E-2</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R9" s="46" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S9" s="14"/>
       <c r="T9" s="14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -23949,13 +24009,13 @@
         <v>88</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F10" s="41">
         <v>44929</v>
@@ -23976,23 +24036,23 @@
       <c r="T10" s="15"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="47" t="s">
-        <v>98</v>
+      <c r="B11" s="52" t="s">
+        <v>168</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F11" s="42">
         <v>44929</v>
       </c>
       <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -24007,21 +24067,21 @@
       <c r="T11" s="19"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="48"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F12" s="43">
         <v>44929</v>
       </c>
       <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
@@ -24036,19 +24096,19 @@
       <c r="T12" s="23"/>
     </row>
     <row r="13" spans="2:20" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F13" s="44">
         <v>44929</v>
       </c>
       <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
@@ -24063,17 +24123,17 @@
       <c r="T13" s="27"/>
     </row>
     <row r="14" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B14" s="47" t="s">
-        <v>99</v>
+      <c r="B14" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F14" s="42">
         <v>44929</v>
@@ -24094,15 +24154,15 @@
       <c r="T14" s="19"/>
     </row>
     <row r="15" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B15" s="48"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F15" s="43">
         <v>44929</v>
@@ -24123,13 +24183,13 @@
       <c r="T15" s="23"/>
     </row>
     <row r="16" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B16" s="49"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F16" s="44">
         <v>44929</v>
@@ -24150,17 +24210,17 @@
       <c r="T16" s="27"/>
     </row>
     <row r="17" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B17" s="13" t="s">
-        <v>94</v>
+      <c r="B17" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F17" s="41">
         <v>44929</v>
@@ -24181,23 +24241,23 @@
       <c r="T17" s="15"/>
     </row>
     <row r="18" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B18" s="13" t="s">
-        <v>96</v>
+      <c r="B18" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F18" s="41">
         <v>44929</v>
       </c>
       <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
@@ -24222,17 +24282,17 @@
       <c r="T18" s="14"/>
     </row>
     <row r="19" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B19" s="13" t="s">
-        <v>94</v>
+      <c r="B19" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F19" s="41">
         <v>44929</v>
@@ -24253,23 +24313,23 @@
       <c r="T19" s="15"/>
     </row>
     <row r="20" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B20" s="13" t="s">
-        <v>96</v>
+      <c r="B20" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F20" s="41">
         <v>44929</v>
       </c>
       <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
@@ -24294,23 +24354,23 @@
       <c r="T20" s="14"/>
     </row>
     <row r="21" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B21" s="13" t="s">
-        <v>96</v>
+      <c r="B21" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F21" s="41">
         <v>44929</v>
       </c>
       <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -24335,17 +24395,17 @@
       <c r="T21" s="14"/>
     </row>
     <row r="22" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B22" s="13" t="s">
-        <v>94</v>
+      <c r="B22" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F22" s="41">
         <v>44929</v>
@@ -24366,23 +24426,23 @@
       <c r="T22" s="15"/>
     </row>
     <row r="23" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B23" s="13" t="s">
-        <v>96</v>
+      <c r="B23" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F23" s="41">
         <v>44929</v>
       </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="15"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
@@ -24407,23 +24467,23 @@
       <c r="T23" s="14"/>
     </row>
     <row r="24" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B24" s="13" t="s">
-        <v>96</v>
+      <c r="B24" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F24" s="41">
         <v>44929</v>
       </c>
       <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="15"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
@@ -24448,17 +24508,17 @@
       <c r="T24" s="14"/>
     </row>
     <row r="25" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B25" s="47" t="s">
-        <v>99</v>
+      <c r="B25" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F25" s="42">
         <v>44929</v>
@@ -24479,15 +24539,15 @@
       <c r="T25" s="19"/>
     </row>
     <row r="26" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B26" s="48"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F26" s="43">
         <v>44929</v>
@@ -24508,13 +24568,13 @@
       <c r="T26" s="23"/>
     </row>
     <row r="27" spans="2:20" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B27" s="49"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F27" s="44">
         <v>44929</v>
@@ -24535,17 +24595,17 @@
       <c r="T27" s="27"/>
     </row>
     <row r="28" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B28" s="13" t="s">
-        <v>94</v>
+      <c r="B28" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F28" s="41">
         <v>44929</v>
@@ -24566,23 +24626,23 @@
       <c r="T28" s="15"/>
     </row>
     <row r="29" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B29" s="13" t="s">
-        <v>96</v>
+      <c r="B29" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F29" s="41">
         <v>44929</v>
       </c>
       <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="15"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
@@ -24607,23 +24667,23 @@
       <c r="T29" s="14"/>
     </row>
     <row r="30" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B30" s="13" t="s">
-        <v>96</v>
+      <c r="B30" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F30" s="41">
         <v>44929</v>
       </c>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="15"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
@@ -24648,17 +24708,17 @@
       <c r="T30" s="14"/>
     </row>
     <row r="31" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B31" s="13" t="s">
-        <v>94</v>
+      <c r="B31" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F31" s="41">
         <v>44929</v>
@@ -24679,23 +24739,23 @@
       <c r="T31" s="15"/>
     </row>
     <row r="32" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B32" s="13" t="s">
-        <v>96</v>
+      <c r="B32" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F32" s="41">
         <v>44929</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="15"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -24720,23 +24780,23 @@
       <c r="T32" s="14"/>
     </row>
     <row r="33" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B33" s="13" t="s">
-        <v>96</v>
+      <c r="B33" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F33" s="41">
         <v>44929</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="H33" s="15"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
@@ -24761,23 +24821,23 @@
       <c r="T33" s="14"/>
     </row>
     <row r="34" spans="2:20" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B34" s="13" t="s">
-        <v>96</v>
+      <c r="B34" s="56" t="s">
+        <v>167</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F34" s="41">
         <v>44929</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="H34" s="15"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -24815,7 +24875,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O35" s="14">
         <f ca="1">SQRT(SUM($P$4:OFFSET($P35,-1,0)))</f>
@@ -24841,7 +24901,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="14" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="O36" s="14">
         <v>6</v>
@@ -45097,7 +45157,7 @@
       <c r="T1000" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="I2:L2"/>
@@ -45105,50 +45165,55 @@
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <conditionalFormatting sqref="E4:F4 E8:F8 E17:F24 E28:F34 E10:F10">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:AG4 P10:AG10 G4 G10">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>C9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>D9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 M4:N4 I10:J10 M10:N10">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 H10">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F19:F34" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(F19))), AND(ISNUMBER(F19), LEFT(CELL("format", F19))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B5 B28:B34 B14 B17:B25 B8:B11" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4 B10" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"カテゴリ,　要求,　親要求,　　子要求,　　　仕様グループ,　　　　仕様"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18 G20:G21 G23:G24 G29:G30 G32:G34 G9" xr:uid="{3BD7A4E9-42B5-4F94-A4D3-FF2E845CBCF4}">
       <formula1>"済"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9 H18 H20:H21 H23:H24 H29:H30 H32:H34" xr:uid="{ED882FB3-B28A-4C6B-AF06-D7780F42C163}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5 H11" xr:uid="{ED882FB3-B28A-4C6B-AF06-D7780F42C163}">
       <formula1>"高,中,低"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B34" xr:uid="{BECB5049-2687-4E9E-912D-A9947792FFAF}">
+      <formula1>"カテゴリ,要求,親要求,子要求,仕様グループ,仕様"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs: update req spec xlsx
</commit_message>
<xml_diff>
--- a/sample_repo/doc/dev/RequirementsSpecification.xlsx
+++ b/sample_repo/doc/dev/RequirementsSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\foox\workspace\documentation_templates\sample_repo\doc\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1484A4C-361E-44D9-A8DD-93A6D0D5A0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CABAC67-6A87-422C-8DDE-74002BD58BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="6495" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="173">
   <si>
     <t>説明</t>
   </si>
@@ -443,15 +443,6 @@
     <t>VSRCH.1.2-SRT.1</t>
   </si>
   <si>
-    <t>マッチしたキーワードの数が多い順にソートする</t>
-  </si>
-  <si>
-    <t>VSRCH.1.2-SRT.2</t>
-  </si>
-  <si>
-    <t>マッチしたキーワードの数が同じ場合は動画の投稿日時が新しい順にソートする</t>
-  </si>
-  <si>
     <t>VSRCH.1.2-UI</t>
   </si>
   <si>
@@ -461,14 +452,6 @@
     <t>VSRCH.1.2-UI.1</t>
   </si>
   <si>
-    <t>ソートされた順で動画ごとに以下を表示する
-・サムネイル
-・タイトル
-・チャンネル名
-・再生数
-・投稿日時</t>
-  </si>
-  <si>
     <t>VSRCH.1.2-UI.2</t>
   </si>
   <si>
@@ -476,9 +459,6 @@
   </si>
   <si>
     <t>VSRCH.1.2-UI.3</t>
-  </si>
-  <si>
-    <t>チャンネル名は動画再生画面に遷移するリンクにする</t>
   </si>
   <si>
     <t>バッファ</t>
@@ -607,6 +587,38 @@
     <rPh sb="30" eb="32">
       <t>ヨウキュウ</t>
     </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ソートされた順で動画ごとに以下を表示する
+・サムネイル
+・タイトル
+・チャンネル名
+・再生数
+・投稿日時</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>マッチしたキーワードの数が多い順および動画の投稿日時が新しい順にソートする</t>
+    <rPh sb="19" eb="21">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ニチジ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ジュン</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>チャンネル名はチャンネル画面に遷移するリンクにする</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -1105,6 +1117,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
@@ -1114,14 +1132,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
@@ -1140,40 +1159,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="BIZ UDPゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1286,6 +1279,25 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="BIZ UDPゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1300,7 +1312,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5C39AB2-E5D6-4B94-B72A-F5713666773B}" name="ステータステーブル" displayName="ステータステーブル" ref="B2:B7" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5C39AB2-E5D6-4B94-B72A-F5713666773B}" name="ステータステーブル" displayName="ステータステーブル" ref="B2:B7" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="B2:B7" xr:uid="{E5C39AB2-E5D6-4B94-B72A-F5713666773B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{FB9C9B62-A0AF-4833-8546-3E9623879AB0}" name="ステータス"/>
@@ -1825,7 +1837,7 @@
     <row r="53" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2490,7 +2502,7 @@
     </row>
     <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B81" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2540,12 +2552,12 @@
     </row>
     <row r="96" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B96" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B97" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2617,23 +2629,23 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="55" t="s">
-        <v>171</v>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="68" t="s">
+        <v>166</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="58" t="s">
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="57"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="61"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
@@ -2652,31 +2664,31 @@
         <v>70</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
-      <c r="I3" s="65" t="s">
+      <c r="I3" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="66" t="s">
+      <c r="L3" s="53" t="s">
         <v>74</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>75</v>
@@ -2718,8 +2730,8 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="59" t="s">
-        <v>151</v>
+      <c r="B5" s="62" t="s">
+        <v>146</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>82</v>
@@ -2730,21 +2742,21 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="62"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="19"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
     </row>
     <row r="6" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="60"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="20" t="s">
         <v>83</v>
       </c>
@@ -2754,21 +2766,21 @@
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="63"/>
+      <c r="H6" s="66"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
     <row r="7" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="61"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
@@ -2776,14 +2788,14 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="64"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="27"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
@@ -2791,7 +2803,7 @@
     </row>
     <row r="8" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="B8" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>84</v>
@@ -2817,7 +2829,7 @@
     </row>
     <row r="9" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="B9" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>85</v>
@@ -2874,8 +2886,8 @@
       <c r="S10" s="14"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="59" t="s">
-        <v>154</v>
+      <c r="B11" s="62" t="s">
+        <v>149</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>82</v>
@@ -2886,21 +2898,21 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
     </row>
     <row r="12" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="60"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="20" t="s">
         <v>83</v>
       </c>
@@ -2910,21 +2922,21 @@
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="63"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="23"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
     <row r="13" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="61"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="24" t="s">
         <v>0</v>
       </c>
@@ -2932,22 +2944,22 @@
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="64"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="26"/>
       <c r="L13" s="27"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B14" s="52" t="s">
-        <v>155</v>
+      <c r="B14" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>86</v>
@@ -2972,7 +2984,7 @@
       <c r="S14" s="18"/>
     </row>
     <row r="15" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B15" s="53"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="20" t="s">
         <v>83</v>
       </c>
@@ -2996,7 +3008,7 @@
       <c r="S15" s="22"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B16" s="54"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="24" t="s">
         <v>0</v>
       </c>
@@ -3019,7 +3031,7 @@
     </row>
     <row r="17" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B17" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>87</v>
@@ -3045,7 +3057,7 @@
     </row>
     <row r="18" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B18" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>85</v>
@@ -3085,7 +3097,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
       <c r="J19" s="31" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K19" s="32">
         <f ca="1">SQRT(SUM($L$4:OFFSET($L19,-1,0)))</f>
@@ -3110,7 +3122,7 @@
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
       <c r="J20" s="31" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K20" s="32">
         <f ca="1">CEILING(SUM($K$4:OFFSET($K20,-1,0)),1)</f>
@@ -22744,27 +22756,27 @@
   </mergeCells>
   <phoneticPr fontId="6"/>
   <conditionalFormatting sqref="E4:F4 E10:F10 I4:O4 I10:O10">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H4 G10:H10">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>C9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>C18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:AG4 P10:AG10">
-    <cfRule type="expression" dxfId="10" priority="23">
+    <cfRule type="expression" dxfId="9" priority="23">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22795,7 +22807,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:S1000"/>
+  <dimension ref="B1:S999"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
@@ -22851,23 +22863,23 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="55" t="s">
-        <v>171</v>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="68" t="s">
+        <v>166</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="58" t="s">
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="57"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="61"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
@@ -22886,10 +22898,10 @@
         <v>70</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>71</v>
@@ -22904,13 +22916,13 @@
         <v>74</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>88</v>
@@ -22956,8 +22968,8 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="59" t="s">
-        <v>151</v>
+      <c r="B5" s="62" t="s">
+        <v>146</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>95</v>
@@ -22972,27 +22984,27 @@
         <v>44929</v>
       </c>
       <c r="G5" s="18"/>
-      <c r="H5" s="62" t="s">
-        <v>156</v>
+      <c r="H5" s="65" t="s">
+        <v>151</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="19"/>
-      <c r="M5" s="62" t="s">
-        <v>172</v>
+      <c r="M5" s="65" t="s">
+        <v>167</v>
       </c>
-      <c r="N5" s="62" t="s">
-        <v>172</v>
+      <c r="N5" s="65" t="s">
+        <v>167</v>
       </c>
-      <c r="O5" s="62"/>
+      <c r="O5" s="65"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
     </row>
     <row r="6" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="60"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="20" t="s">
         <v>83</v>
       </c>
@@ -23006,21 +23018,21 @@
         <v>44929</v>
       </c>
       <c r="G6" s="22"/>
-      <c r="H6" s="63"/>
+      <c r="H6" s="66"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
     <row r="7" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="61"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
@@ -23032,14 +23044,14 @@
         <v>44929</v>
       </c>
       <c r="G7" s="26"/>
-      <c r="H7" s="64"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="27"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
@@ -23047,7 +23059,7 @@
     </row>
     <row r="8" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="B8" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>98</v>
@@ -23077,7 +23089,7 @@
     </row>
     <row r="9" spans="2:19" ht="30" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="B9" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>100</v>
@@ -23092,7 +23104,7 @@
         <v>44929</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="13">
@@ -23116,7 +23128,7 @@
         <v>102</v>
       </c>
       <c r="Q9" s="45" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="R9" s="13"/>
       <c r="S9" s="13" t="s">
@@ -23154,8 +23166,8 @@
       <c r="S10" s="14"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="59" t="s">
-        <v>154</v>
+      <c r="B11" s="62" t="s">
+        <v>149</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>106</v>
@@ -23170,25 +23182,25 @@
         <v>44929</v>
       </c>
       <c r="G11" s="18"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="62" t="s">
-        <v>172</v>
+      <c r="M11" s="65" t="s">
+        <v>167</v>
       </c>
-      <c r="N11" s="62" t="s">
-        <v>172</v>
+      <c r="N11" s="65" t="s">
+        <v>167</v>
       </c>
-      <c r="O11" s="62"/>
+      <c r="O11" s="65"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
     </row>
     <row r="12" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="60"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="20" t="s">
         <v>83</v>
       </c>
@@ -23202,21 +23214,21 @@
         <v>44929</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="63"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="23"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
     <row r="13" spans="2:19" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="61"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="24" t="s">
         <v>0</v>
       </c>
@@ -23228,22 +23240,22 @@
         <v>44929</v>
       </c>
       <c r="G13" s="26"/>
-      <c r="H13" s="64"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="26"/>
       <c r="L13" s="27"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B14" s="52" t="s">
-        <v>155</v>
+      <c r="B14" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>109</v>
@@ -23272,7 +23284,7 @@
       <c r="S14" s="18"/>
     </row>
     <row r="15" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B15" s="53"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="20" t="s">
         <v>83</v>
       </c>
@@ -23300,7 +23312,7 @@
       <c r="S15" s="22"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B16" s="54"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="24" t="s">
         <v>0</v>
       </c>
@@ -23327,7 +23339,7 @@
     </row>
     <row r="17" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B17" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>112</v>
@@ -23357,7 +23369,7 @@
     </row>
     <row r="18" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B18" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>114</v>
@@ -23372,7 +23384,7 @@
         <v>44929</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="13">
@@ -23399,7 +23411,7 @@
     </row>
     <row r="19" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B19" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>116</v>
@@ -23429,7 +23441,7 @@
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B20" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>118</v>
@@ -23444,7 +23456,7 @@
         <v>44929</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="13">
@@ -23471,7 +23483,7 @@
     </row>
     <row r="21" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B21" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>120</v>
@@ -23486,7 +23498,7 @@
         <v>44929</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="13">
@@ -23513,7 +23525,7 @@
     </row>
     <row r="22" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B22" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>122</v>
@@ -23543,7 +23555,7 @@
     </row>
     <row r="23" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B23" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>124</v>
@@ -23558,7 +23570,7 @@
         <v>44929</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="13">
@@ -23585,7 +23597,7 @@
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B24" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>126</v>
@@ -23600,7 +23612,7 @@
         <v>44929</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="13">
@@ -23626,8 +23638,8 @@
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B25" s="52" t="s">
-        <v>155</v>
+      <c r="B25" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>128</v>
@@ -23656,7 +23668,7 @@
       <c r="S25" s="18"/>
     </row>
     <row r="26" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B26" s="53"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="20" t="s">
         <v>83</v>
       </c>
@@ -23684,7 +23696,7 @@
       <c r="S26" s="22"/>
     </row>
     <row r="27" spans="2:19" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="B27" s="54"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="24" t="s">
         <v>0</v>
       </c>
@@ -23711,7 +23723,7 @@
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B28" s="47" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>131</v>
@@ -23741,13 +23753,13 @@
     </row>
     <row r="29" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B29" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>94</v>
@@ -23756,7 +23768,7 @@
         <v>44929</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="13">
@@ -23766,11 +23778,11 @@
         <v>1</v>
       </c>
       <c r="K29" s="13">
-        <f t="shared" ref="K29:K30" si="4">(I29+J29)/2</f>
+        <f t="shared" ref="K29" si="4">(I29+J29)/2</f>
         <v>0.75</v>
       </c>
       <c r="L29" s="28">
-        <f t="shared" ref="L29:L30" si="5">(J29-K29)^2</f>
+        <f t="shared" ref="L29" si="5">(J29-K29)^2</f>
         <v>6.25E-2</v>
       </c>
       <c r="M29" s="15"/>
@@ -23782,14 +23794,14 @@
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B30" s="48" t="s">
-        <v>153</v>
+      <c r="B30" s="47" t="s">
+        <v>147</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>94</v>
@@ -23797,41 +23809,29 @@
       <c r="F30" s="40">
         <v>44929</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>160</v>
-      </c>
+      <c r="G30" s="14"/>
       <c r="H30" s="14"/>
-      <c r="I30" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="J30" s="13">
-        <v>1</v>
-      </c>
-      <c r="K30" s="13">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="L30" s="28">
-        <f t="shared" si="5"/>
-        <v>6.25E-2</v>
-      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-    </row>
-    <row r="31" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B31" s="47" t="s">
-        <v>152</v>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+    </row>
+    <row r="31" spans="2:19" ht="72" outlineLevel="3" x14ac:dyDescent="0.15">
+      <c r="B31" s="48" t="s">
+        <v>148</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>94</v>
@@ -23839,29 +23839,41 @@
       <c r="F31" s="40">
         <v>44929</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="13" t="s">
+        <v>155</v>
+      </c>
       <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="15"/>
+      <c r="I31" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="J31" s="13">
+        <v>1</v>
+      </c>
+      <c r="K31" s="13">
+        <f t="shared" ref="K31:K33" si="6">(I31+J31)/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="L31" s="28">
+        <f t="shared" ref="L31:L33" si="7">(J31-K31)^2</f>
+        <v>6.25E-2</v>
+      </c>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B32" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>94</v>
@@ -23870,22 +23882,22 @@
         <v>44929</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H32" s="14"/>
       <c r="I32" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="J32" s="13">
         <v>0.5</v>
       </c>
-      <c r="J32" s="13">
-        <v>1</v>
-      </c>
       <c r="K32" s="13">
-        <f t="shared" ref="K32:K34" si="6">(I32+J32)/2</f>
-        <v>0.75</v>
+        <f t="shared" si="6"/>
+        <v>0.375</v>
       </c>
       <c r="L32" s="28">
-        <f t="shared" ref="L32:L34" si="7">(J32-K32)^2</f>
-        <v>6.25E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.5625E-2</v>
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
@@ -23897,13 +23909,13 @@
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
       <c r="B33" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>94</v>
@@ -23912,7 +23924,7 @@
         <v>44929</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H33" s="14"/>
       <c r="I33" s="13">
@@ -23937,47 +23949,30 @@
       <c r="R33" s="13"/>
       <c r="S33" s="13"/>
     </row>
-    <row r="34" spans="2:19" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.15">
-      <c r="B34" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F34" s="40">
-        <v>44929</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="H34" s="14"/>
-      <c r="I34" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="J34" s="13">
-        <v>0.5</v>
+    <row r="34" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="K34" s="13">
-        <f t="shared" si="6"/>
-        <v>0.375</v>
+        <f ca="1">SQRT(SUM($L$4:OFFSET($L34,-1,0)))</f>
+        <v>0.55509008277936289</v>
       </c>
-      <c r="L34" s="28">
-        <f t="shared" si="7"/>
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="7"/>
@@ -23989,13 +23984,13 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
-      <c r="K35" s="13">
-        <f ca="1">SQRT(SUM($L$4:OFFSET($L35,-1,0)))</f>
-        <v>0.60878978309429599</v>
+      <c r="K35" s="32">
+        <f ca="1">CEILING(SUM($K$4:OFFSET($K35,-1,0)),1)</f>
+        <v>6</v>
       </c>
-      <c r="L35" s="30"/>
+      <c r="L35" s="44"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -24013,14 +24008,9 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="K36" s="32">
-        <f ca="1">CEILING(SUM($K$4:OFFSET($K36,-1,0)),1)</f>
-        <v>6</v>
-      </c>
-      <c r="L36" s="44"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
@@ -24193,8 +24183,8 @@
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="38"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
@@ -43289,26 +43279,6 @@
       <c r="R999" s="8"/>
       <c r="S999" s="8"/>
     </row>
-    <row r="1000" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="7"/>
-      <c r="D1000" s="38"/>
-      <c r="E1000" s="8"/>
-      <c r="F1000" s="8"/>
-      <c r="G1000" s="8"/>
-      <c r="H1000" s="8"/>
-      <c r="I1000" s="8"/>
-      <c r="J1000" s="8"/>
-      <c r="K1000" s="8"/>
-      <c r="L1000" s="8"/>
-      <c r="M1000" s="8"/>
-      <c r="N1000" s="8"/>
-      <c r="O1000" s="8"/>
-      <c r="P1000" s="8"/>
-      <c r="Q1000" s="8"/>
-      <c r="R1000" s="8"/>
-      <c r="S1000" s="8"/>
-    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B14:B16"/>
@@ -43328,69 +43298,69 @@
     <mergeCell ref="O11:O13"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
-  <conditionalFormatting sqref="E4:F4 E8:F8 E17:F24 E28:F34 E10:F10 I10:J10">
-    <cfRule type="expression" dxfId="9" priority="6">
+  <conditionalFormatting sqref="E4:F4 E8:F8 E17:F24 E10:F10 I10:J10 E28:F33">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4 G10">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>C9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>D9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>G4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 H10">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10 L4">
-    <cfRule type="expression" dxfId="3" priority="24">
+    <cfRule type="expression" dxfId="2" priority="24">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:O4 M10:O10">
-    <cfRule type="expression" dxfId="2" priority="27">
+    <cfRule type="expression" dxfId="1" priority="27">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:AF4 P10:AF10">
-    <cfRule type="expression" dxfId="1" priority="29">
+    <cfRule type="expression" dxfId="0" priority="29">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F19:F34" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(F19))), AND(ISNUMBER(F19), LEFT(CELL("format", F19))="D"))</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4 B10" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"カテゴリ,　要求,　親要求,　　子要求,　　　仕様グループ,　　　　仕様"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5 H11" xr:uid="{ED882FB3-B28A-4C6B-AF06-D7780F42C163}">
       <formula1>"高,中,低"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B34" xr:uid="{BECB5049-2687-4E9E-912D-A9947792FFAF}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B33" xr:uid="{BECB5049-2687-4E9E-912D-A9947792FFAF}">
       <formula1>"カテゴリ,要求,親要求,子要求,仕様グループ,仕様"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9 G18 G29:G30 G20:G21 G23:G24 G32:G34" xr:uid="{928B4FB5-991A-42F4-9AA4-0FB8E9E0BB5F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9 G18 G29 G20:G21 G23:G24 G31:G33" xr:uid="{928B4FB5-991A-42F4-9AA4-0FB8E9E0BB5F}">
       <formula1>ステータス</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:O7 M11:O13" xr:uid="{0D2DBA87-525A-4610-8B60-3D627CBBE232}">
       <formula1>"〇"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F19:F33" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(F19))), AND(ISNUMBER(F19), LEFT(CELL("format", F19))="D"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43411,32 +43381,32 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="49" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>